<commit_message>
Feat/board item import (#798)
close erxes/erxes#2056
</commit_message>
<xml_diff>
--- a/src/private/importTemplates/company_template.xlsx
+++ b/src/private/importTemplates/company_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">primaryName</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customersPrimaryNames</t>
   </si>
 </sst>
 </file>
@@ -144,20 +147,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="9" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="0" width="8.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -188,6 +194,9 @@
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>